<commit_message>
Added reset event for loop sub-commands. Fixed calculation of cross product. Added reset of location for Y axis (fork-lift). Syntax fixes in test file.
</commit_message>
<xml_diff>
--- a/test/DotCrossProducts.xlsx
+++ b/test/DotCrossProducts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\source\repos\CommandRunner\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B55A2E-BA54-451E-9354-C6FC030B3B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEA23F6-CABD-4103-8FAB-AEB9E41F5E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="624" yWindow="624" windowWidth="17280" windowHeight="9468" xr2:uid="{FCF57B52-49C1-4DF5-A408-2D8B16D4A2EE}"/>
   </bookViews>
@@ -33,28 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -453,21 +431,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0481DA76-E960-45EC-B126-5E3DF8B5A025}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5546875" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -507,23 +485,23 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <f>SIN(RADIANS(A2))</f>
+        <f t="shared" ref="C2:C9" si="0">SIN(RADIANS(A2))</f>
         <v>0</v>
       </c>
       <c r="D2">
-        <f>COS(RADIANS(A2))</f>
+        <f t="shared" ref="D2:D9" si="1">COS(RADIANS(A2))</f>
         <v>1</v>
       </c>
       <c r="E2">
-        <f>SIN(RADIANS(B2))</f>
+        <f t="shared" ref="E2:E9" si="2">SIN(RADIANS(B2))</f>
         <v>0.17364817766693033</v>
       </c>
       <c r="F2">
-        <f>COS(RADIANS(B2))</f>
+        <f t="shared" ref="F2:F9" si="3">COS(RADIANS(B2))</f>
         <v>0.98480775301220802</v>
       </c>
       <c r="G2">
-        <f>+C2*F2-D2*E2</f>
+        <f t="shared" ref="G2:G9" si="4">+C2*F2-D2*E2</f>
         <v>-0.17364817766693033</v>
       </c>
       <c r="H2">
@@ -531,7 +509,7 @@
         <v>0.98480775301220802</v>
       </c>
       <c r="I2" t="str">
-        <f>IF(G2&lt;0, "CW", "CCW")</f>
+        <f t="shared" ref="I2:I9" si="5">IF(G2&lt;0, "CW", "CCW")</f>
         <v>CW</v>
       </c>
       <c r="J2">
@@ -539,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -547,39 +525,39 @@
         <v>190</v>
       </c>
       <c r="C3">
-        <f>SIN(RADIANS(A3))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D3">
-        <f>COS(RADIANS(A3))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E3">
-        <f>SIN(RADIANS(B3))</f>
+        <f t="shared" si="2"/>
         <v>-0.17364817766693047</v>
       </c>
       <c r="F3">
-        <f>COS(RADIANS(B3))</f>
+        <f t="shared" si="3"/>
         <v>-0.98480775301220802</v>
       </c>
       <c r="G3">
-        <f>+C3*F3-D3*E3</f>
+        <f t="shared" si="4"/>
         <v>0.17364817766693047</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H8" si="0">+C3*E3+D3*F3</f>
+        <f t="shared" ref="H3:H9" si="6">+C3*E3+D3*F3</f>
         <v>-0.98480775301220802</v>
       </c>
       <c r="I3" t="str">
-        <f>IF(G3&lt;0, "CW", "CCW")</f>
+        <f t="shared" si="5"/>
         <v>CCW</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J8" si="1">-DEGREES(ATAN2(H3,G3))</f>
+        <f t="shared" ref="J3:J9" si="7">-DEGREES(ATAN2(H3,G3))</f>
         <v>-169.99999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>170</v>
       </c>
@@ -587,39 +565,39 @@
         <v>190</v>
       </c>
       <c r="C4">
-        <f>SIN(RADIANS(A4))</f>
+        <f t="shared" si="0"/>
         <v>0.17364817766693028</v>
       </c>
       <c r="D4">
-        <f>COS(RADIANS(A4))</f>
+        <f t="shared" si="1"/>
         <v>-0.98480775301220802</v>
       </c>
       <c r="E4">
-        <f>SIN(RADIANS(B4))</f>
+        <f t="shared" si="2"/>
         <v>-0.17364817766693047</v>
       </c>
       <c r="F4">
-        <f>COS(RADIANS(B4))</f>
+        <f t="shared" si="3"/>
         <v>-0.98480775301220802</v>
       </c>
       <c r="G4">
-        <f>+C4*F4-D4*E4</f>
+        <f t="shared" si="4"/>
         <v>-0.34202014332566877</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.93969262078590832</v>
       </c>
       <c r="I4" t="str">
-        <f>IF(G4&lt;0, "CW", "CCW")</f>
+        <f t="shared" si="5"/>
         <v>CW</v>
       </c>
       <c r="J4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>20.000000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>80</v>
       </c>
@@ -627,39 +605,39 @@
         <v>280</v>
       </c>
       <c r="C5">
-        <f>SIN(RADIANS(A5))</f>
+        <f t="shared" si="0"/>
         <v>0.98480775301220802</v>
       </c>
       <c r="D5">
-        <f>COS(RADIANS(A5))</f>
+        <f t="shared" si="1"/>
         <v>0.17364817766693041</v>
       </c>
       <c r="E5">
-        <f>SIN(RADIANS(B5))</f>
+        <f t="shared" si="2"/>
         <v>-0.98480775301220813</v>
       </c>
       <c r="F5">
-        <f>COS(RADIANS(B5))</f>
+        <f t="shared" si="3"/>
         <v>0.17364817766692997</v>
       </c>
       <c r="G5">
-        <f>+C5*F5-D5*E5</f>
+        <f t="shared" si="4"/>
         <v>0.34202014332566844</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-0.93969262078590843</v>
       </c>
       <c r="I5" t="str">
-        <f>IF(G5&lt;0, "CW", "CCW")</f>
+        <f t="shared" si="5"/>
         <v>CCW</v>
       </c>
       <c r="J5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>-160.00000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -667,39 +645,39 @@
         <v>355</v>
       </c>
       <c r="C6">
-        <f>SIN(RADIANS(A6))</f>
+        <f t="shared" si="0"/>
         <v>8.7155742747658166E-2</v>
       </c>
       <c r="D6">
-        <f>COS(RADIANS(A6))</f>
+        <f t="shared" si="1"/>
         <v>0.99619469809174555</v>
       </c>
       <c r="E6">
-        <f>SIN(RADIANS(B6))</f>
+        <f t="shared" si="2"/>
         <v>-8.7155742747658319E-2</v>
       </c>
       <c r="F6">
-        <f>COS(RADIANS(B6))</f>
+        <f t="shared" si="3"/>
         <v>0.99619469809174555</v>
       </c>
       <c r="G6">
-        <f>+C6*F6-D6*E6</f>
+        <f t="shared" si="4"/>
         <v>0.17364817766693047</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.98480775301220813</v>
       </c>
       <c r="I6" t="str">
-        <f>IF(G6&lt;0, "CW", "CCW")</f>
+        <f t="shared" si="5"/>
         <v>CCW</v>
       </c>
       <c r="J6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>-10.000000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>355</v>
       </c>
@@ -707,39 +685,39 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <f>SIN(RADIANS(A7))</f>
+        <f t="shared" si="0"/>
         <v>-8.7155742747658319E-2</v>
       </c>
       <c r="D7">
-        <f>COS(RADIANS(A7))</f>
+        <f t="shared" si="1"/>
         <v>0.99619469809174555</v>
       </c>
       <c r="E7">
-        <f>SIN(RADIANS(B7))</f>
+        <f t="shared" si="2"/>
         <v>8.7155742747658166E-2</v>
       </c>
       <c r="F7">
-        <f>COS(RADIANS(B7))</f>
+        <f t="shared" si="3"/>
         <v>0.99619469809174555</v>
       </c>
       <c r="G7">
-        <f>+C7*F7-D7*E7</f>
+        <f t="shared" si="4"/>
         <v>-0.17364817766693047</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.98480775301220813</v>
       </c>
       <c r="I7" t="str">
-        <f>IF(G7&lt;0, "CW", "CCW")</f>
+        <f t="shared" si="5"/>
         <v>CW</v>
       </c>
       <c r="J7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>10.000000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>90</v>
       </c>
@@ -747,50 +725,86 @@
         <v>206</v>
       </c>
       <c r="C8">
-        <f>SIN(RADIANS(A8))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D8">
-        <f>COS(RADIANS(A8))</f>
+        <f t="shared" si="1"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="E8">
-        <f>SIN(RADIANS(B8))</f>
+        <f t="shared" si="2"/>
         <v>-0.43837114678907746</v>
       </c>
       <c r="F8">
-        <f>COS(RADIANS(B8))</f>
+        <f t="shared" si="3"/>
         <v>-0.89879404629916693</v>
       </c>
       <c r="G8">
-        <f>+C8*F8-D8*E8</f>
+        <f t="shared" si="4"/>
         <v>-0.89879404629916693</v>
       </c>
       <c r="H8">
+        <f t="shared" si="6"/>
+        <v>-0.43837114678907751</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="5"/>
+        <v>CW</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="7"/>
+        <v>116.00000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>180</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="0"/>
-        <v>-0.43837114678907751</v>
-      </c>
-      <c r="I8" t="str">
-        <f>IF(G8&lt;0, "CW", "CCW")</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>-0.70710678118654757</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="6"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="5"/>
         <v>CW</v>
       </c>
-      <c r="J8">
-        <f t="shared" si="1"/>
-        <v>116.00000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="J9">
+        <f t="shared" si="7"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C9" t="e" cm="1">
-        <f t="array" ref="C9">atan2</f>
-        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" xr:uid="{D55C66E4-AAC1-4B29-8A24-328D55A1F79E}"/>
+    <hyperlink ref="A10" r:id="rId1" xr:uid="{D55C66E4-AAC1-4B29-8A24-328D55A1F79E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>